<commit_message>
Update California Ballot Measures Nov 2022.xlsx
</commit_message>
<xml_diff>
--- a/003_data/001_raw-data/Ballot Measures/California Ballot Measures Nov 2022.xlsx
+++ b/003_data/001_raw-data/Ballot Measures/California Ballot Measures Nov 2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\soswebdev\transmit\cdn\elections\sov\2022-general\sov\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udghealthcare-my.sharepoint.com/personal/iris_lin_inizioevoke_com/Documents/Documents/Scripts_2024/milestone_1/003_data/001_raw-data/Ballot Measures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84F1D84A-0C21-4CE1-BA15-9E370FB789A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{84F1D84A-0C21-4CE1-BA15-9E370FB789A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21B749C5-A159-4749-BD0D-41BA5ADEADEC}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5670" windowWidth="38640" windowHeight="21240"/>
+    <workbookView minimized="1" xWindow="9270" yWindow="2790" windowWidth="2220" windowHeight="980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOV Ballot Measures Export" sheetId="1" r:id="rId1"/>
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -813,9 +813,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -853,7 +853,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -959,7 +959,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1101,21 +1101,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I407"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44873</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>74916</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44873</v>
       </c>
@@ -1202,7 +1205,7 @@
         <v>310131</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44873</v>
       </c>
@@ -1231,7 +1234,7 @@
         <v>404086</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44873</v>
       </c>
@@ -1260,7 +1263,7 @@
         <v>123275</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44873</v>
       </c>
@@ -1289,7 +1292,7 @@
         <v>290746</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44873</v>
       </c>
@@ -1318,7 +1321,7 @@
         <v>224613</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44873</v>
       </c>
@@ -1347,7 +1350,7 @@
         <v>115606</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44873</v>
       </c>
@@ -1376,7 +1379,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44873</v>
       </c>
@@ -1405,7 +1408,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44873</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44873</v>
       </c>
@@ -1463,7 +1466,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>44873</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>44873</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>44873</v>
       </c>
@@ -1550,7 +1553,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>44873</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>9216</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>44873</v>
       </c>
@@ -1608,7 +1611,7 @@
         <v>14314</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>44873</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>16189</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>44873</v>
       </c>
@@ -1666,7 +1669,7 @@
         <v>8767</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>44873</v>
       </c>
@@ -1695,7 +1698,7 @@
         <v>14569</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>44873</v>
       </c>
@@ -1724,7 +1727,7 @@
         <v>12643</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>44873</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>8684</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>44873</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>29072</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>44873</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>48375</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>44873</v>
       </c>
@@ -1840,7 +1843,7 @@
         <v>60169</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>44873</v>
       </c>
@@ -1869,7 +1872,7 @@
         <v>28098</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>44873</v>
       </c>
@@ -1898,7 +1901,7 @@
         <v>54015</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>44873</v>
       </c>
@@ -1927,7 +1930,7 @@
         <v>41716</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>44873</v>
       </c>
@@ -1956,7 +1959,7 @@
         <v>31590</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>44873</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>10266</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>44873</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>15596</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>44873</v>
       </c>
@@ -2043,7 +2046,7 @@
         <v>18405</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>44873</v>
       </c>
@@ -2072,7 +2075,7 @@
         <v>10031</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>44873</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>16440</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>44873</v>
       </c>
@@ -2130,7 +2133,7 @@
         <v>14273</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>44873</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>10090</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>44873</v>
       </c>
@@ -2188,7 +2191,7 @@
         <v>2939</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>44873</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>4190</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>44873</v>
       </c>
@@ -2246,7 +2249,7 @@
         <v>4601</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>44873</v>
       </c>
@@ -2275,7 +2278,7 @@
         <v>2662</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>44873</v>
       </c>
@@ -2304,7 +2307,7 @@
         <v>4213</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>44873</v>
       </c>
@@ -2333,7 +2336,7 @@
         <v>3923</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>44873</v>
       </c>
@@ -2362,7 +2365,7 @@
         <v>2796</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>44873</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>93584</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>44873</v>
       </c>
@@ -2420,7 +2423,7 @@
         <v>261183</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44873</v>
       </c>
@@ -2449,7 +2452,7 @@
         <v>318798</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>44873</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>117236</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>44873</v>
       </c>
@@ -2507,7 +2510,7 @@
         <v>257323</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>44873</v>
       </c>
@@ -2536,7 +2539,7 @@
         <v>209016</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>44873</v>
       </c>
@@ -2565,7 +2568,7 @@
         <v>106801</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>44873</v>
       </c>
@@ -2594,7 +2597,7 @@
         <v>3967</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>44873</v>
       </c>
@@ -2623,7 +2626,7 @@
         <v>5785</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>44873</v>
       </c>
@@ -2652,7 +2655,7 @@
         <v>6935</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>44873</v>
       </c>
@@ -2681,7 +2684,7 @@
         <v>3785</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>44873</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>5481</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>44873</v>
       </c>
@@ -2739,7 +2742,7 @@
         <v>5047</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>44873</v>
       </c>
@@ -2768,7 +2771,7 @@
         <v>4163</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>44873</v>
       </c>
@@ -2797,7 +2800,7 @@
         <v>39853</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>44873</v>
       </c>
@@ -2826,7 +2829,7 @@
         <v>64165</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>44873</v>
       </c>
@@ -2855,7 +2858,7 @@
         <v>74978</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>44873</v>
       </c>
@@ -2884,7 +2887,7 @@
         <v>40459</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>44873</v>
       </c>
@@ -2913,7 +2916,7 @@
         <v>66575</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>44873</v>
       </c>
@@ -2942,7 +2945,7 @@
         <v>56260</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>44873</v>
       </c>
@@ -2971,7 +2974,7 @@
         <v>37382</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>44873</v>
       </c>
@@ -3000,7 +3003,7 @@
         <v>99612</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>44873</v>
       </c>
@@ -3029,7 +3032,7 @@
         <v>158560</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>44873</v>
       </c>
@@ -3058,7 +3061,7 @@
         <v>178652</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>44873</v>
       </c>
@@ -3087,7 +3090,7 @@
         <v>96062</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>44873</v>
       </c>
@@ -3116,7 +3119,7 @@
         <v>156778</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>44873</v>
       </c>
@@ -3145,7 +3148,7 @@
         <v>134749</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>44873</v>
       </c>
@@ -3174,7 +3177,7 @@
         <v>101929</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>44873</v>
       </c>
@@ -3203,7 +3206,7 @@
         <v>4185</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>44873</v>
       </c>
@@ -3232,7 +3235,7 @@
         <v>5932</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>44873</v>
       </c>
@@ -3261,7 +3264,7 @@
         <v>6694</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>44873</v>
       </c>
@@ -3290,7 +3293,7 @@
         <v>4050</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>44873</v>
       </c>
@@ -3319,7 +3322,7 @@
         <v>6349</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>44873</v>
       </c>
@@ -3348,7 +3351,7 @@
         <v>5902</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>44873</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>4231</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>44873</v>
       </c>
@@ -3406,7 +3409,7 @@
         <v>12587</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>44873</v>
       </c>
@@ -3435,7 +3438,7 @@
         <v>31072</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>44873</v>
       </c>
@@ -3464,7 +3467,7 @@
         <v>39419</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>44873</v>
       </c>
@@ -3493,7 +3496,7 @@
         <v>14377</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>44873</v>
       </c>
@@ -3522,7 +3525,7 @@
         <v>31147</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>44873</v>
       </c>
@@ -3551,7 +3554,7 @@
         <v>21048</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>44873</v>
       </c>
@@ -3580,7 +3583,7 @@
         <v>16635</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>44873</v>
       </c>
@@ -3609,7 +3612,7 @@
         <v>13419</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>44873</v>
       </c>
@@ -3638,7 +3641,7 @@
         <v>18723</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>44873</v>
       </c>
@@ -3667,7 +3670,7 @@
         <v>22842</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>44873</v>
       </c>
@@ -3696,7 +3699,7 @@
         <v>10708</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>44873</v>
       </c>
@@ -3725,7 +3728,7 @@
         <v>16598</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>44873</v>
       </c>
@@ -3754,7 +3757,7 @@
         <v>15812</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>44873</v>
       </c>
@@ -3783,7 +3786,7 @@
         <v>12699</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>44873</v>
       </c>
@@ -3812,7 +3815,7 @@
         <v>2883</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>44873</v>
       </c>
@@ -3841,7 +3844,7 @@
         <v>5063</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>44873</v>
       </c>
@@ -3870,7 +3873,7 @@
         <v>6302</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>44873</v>
       </c>
@@ -3899,7 +3902,7 @@
         <v>3009</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>44873</v>
       </c>
@@ -3928,7 +3931,7 @@
         <v>5559</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>44873</v>
       </c>
@@ -3957,7 +3960,7 @@
         <v>4643</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>44873</v>
       </c>
@@ -3986,7 +3989,7 @@
         <v>3086</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>44873</v>
       </c>
@@ -4015,7 +4018,7 @@
         <v>97194</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>44873</v>
       </c>
@@ -4044,7 +4047,7 @@
         <v>127003</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>44873</v>
       </c>
@@ -4073,7 +4076,7 @@
         <v>150976</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>44873</v>
       </c>
@@ -4102,7 +4105,7 @@
         <v>88352</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>44873</v>
       </c>
@@ -4131,7 +4134,7 @@
         <v>135398</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>44873</v>
       </c>
@@ -4160,7 +4163,7 @@
         <v>125382</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>44873</v>
       </c>
@@ -4189,7 +4192,7 @@
         <v>97751</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>44873</v>
       </c>
@@ -4218,7 +4221,7 @@
         <v>14420</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>44873</v>
       </c>
@@ -4247,7 +4250,7 @@
         <v>19413</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>44873</v>
       </c>
@@ -4276,7 +4279,7 @@
         <v>21937</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>44873</v>
       </c>
@@ -4305,7 +4308,7 @@
         <v>12639</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>44873</v>
       </c>
@@ -4334,7 +4337,7 @@
         <v>19572</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>44873</v>
       </c>
@@ -4363,7 +4366,7 @@
         <v>18232</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>44873</v>
       </c>
@@ -4392,7 +4395,7 @@
         <v>14076</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>44873</v>
       </c>
@@ -4421,7 +4424,7 @@
         <v>7432</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>44873</v>
       </c>
@@ -4450,7 +4453,7 @@
         <v>14384</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>44873</v>
       </c>
@@ -4479,7 +4482,7 @@
         <v>17304</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>44873</v>
       </c>
@@ -4508,7 +4511,7 @@
         <v>7486</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>44873</v>
       </c>
@@ -4537,7 +4540,7 @@
         <v>14303</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>44873</v>
       </c>
@@ -4566,7 +4569,7 @@
         <v>12285</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>44873</v>
       </c>
@@ -4595,7 +4598,7 @@
         <v>8409</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>44873</v>
       </c>
@@ -4624,7 +4627,7 @@
         <v>5434</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>44873</v>
       </c>
@@ -4653,7 +4656,7 @@
         <v>6408</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>44873</v>
       </c>
@@ -4682,7 +4685,7 @@
         <v>7469</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>44873</v>
       </c>
@@ -4711,7 +4714,7 @@
         <v>4603</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>44873</v>
       </c>
@@ -4740,7 +4743,7 @@
         <v>6878</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>44873</v>
       </c>
@@ -4769,7 +4772,7 @@
         <v>7243</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>44873</v>
       </c>
@@ -4798,7 +4801,7 @@
         <v>5279</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>44873</v>
       </c>
@@ -4827,7 +4830,7 @@
         <v>635668</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>44873</v>
       </c>
@@ -4856,7 +4859,7 @@
         <v>1472472</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>44873</v>
       </c>
@@ -4885,7 +4888,7 @@
         <v>1869661</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>44873</v>
       </c>
@@ -4914,7 +4917,7 @@
         <v>706529</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>44873</v>
       </c>
@@ -4943,7 +4946,7 @@
         <v>1462984</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>44873</v>
       </c>
@@ -4972,7 +4975,7 @@
         <v>1373773</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>44873</v>
       </c>
@@ -5001,7 +5004,7 @@
         <v>778227</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>44873</v>
       </c>
@@ -5030,7 +5033,7 @@
         <v>19544</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>44873</v>
       </c>
@@ -5059,7 +5062,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>44873</v>
       </c>
@@ -5088,7 +5091,7 @@
         <v>30946</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>44873</v>
       </c>
@@ -5117,7 +5120,7 @@
         <v>17646</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>44873</v>
       </c>
@@ -5146,7 +5149,7 @@
         <v>27475</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>44873</v>
       </c>
@@ -5175,7 +5178,7 @@
         <v>24739</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>44873</v>
       </c>
@@ -5204,7 +5207,7 @@
         <v>18317</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>44873</v>
       </c>
@@ -5233,7 +5236,7 @@
         <v>16872</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>44873</v>
       </c>
@@ -5262,7 +5265,7 @@
         <v>83604</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>44873</v>
       </c>
@@ -5291,7 +5294,7 @@
         <v>99950</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>44873</v>
       </c>
@@ -5320,7 +5323,7 @@
         <v>29745</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>44873</v>
       </c>
@@ -5349,7 +5352,7 @@
         <v>81246</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>44873</v>
       </c>
@@ -5378,7 +5381,7 @@
         <v>59704</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>44873</v>
       </c>
@@ -5407,7 +5410,7 @@
         <v>21737</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>44873</v>
       </c>
@@ -5436,7 +5439,7 @@
         <v>3783</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>44873</v>
       </c>
@@ -5465,7 +5468,7 @@
         <v>5998</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>44873</v>
       </c>
@@ -5494,7 +5497,7 @@
         <v>6877</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>44873</v>
       </c>
@@ -5523,7 +5526,7 @@
         <v>3542</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>44873</v>
       </c>
@@ -5552,7 +5555,7 @@
         <v>5971</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>44873</v>
       </c>
@@ -5581,7 +5584,7 @@
         <v>4955</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>44873</v>
       </c>
@@ -5610,7 +5613,7 @@
         <v>3821</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>44873</v>
       </c>
@@ -5639,7 +5642,7 @@
         <v>7590</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>44873</v>
       </c>
@@ -5668,7 +5671,7 @@
         <v>21589</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>44873</v>
       </c>
@@ -5697,7 +5700,7 @@
         <v>26278</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>44873</v>
       </c>
@@ -5726,7 +5729,7 @@
         <v>8714</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>44873</v>
       </c>
@@ -5755,7 +5758,7 @@
         <v>21027</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>44873</v>
       </c>
@@ -5784,7 +5787,7 @@
         <v>15028</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>44873</v>
       </c>
@@ -5813,7 +5816,7 @@
         <v>9711</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>44873</v>
       </c>
@@ -5842,7 +5845,7 @@
         <v>25237</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>44873</v>
       </c>
@@ -5871,7 +5874,7 @@
         <v>38202</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>44873</v>
       </c>
@@ -5900,7 +5903,7 @@
         <v>44014</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>44873</v>
       </c>
@@ -5929,7 +5932,7 @@
         <v>21514</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>44873</v>
       </c>
@@ -5958,7 +5961,7 @@
         <v>38311</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>44873</v>
       </c>
@@ -5987,7 +5990,7 @@
         <v>33808</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>44873</v>
       </c>
@@ -6016,7 +6019,7 @@
         <v>24423</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>44873</v>
       </c>
@@ -6045,7 +6048,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>44873</v>
       </c>
@@ -6074,7 +6077,7 @@
         <v>2536</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>44873</v>
       </c>
@@ -6103,7 +6106,7 @@
         <v>2899</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>44873</v>
       </c>
@@ -6132,7 +6135,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>44873</v>
       </c>
@@ -6161,7 +6164,7 @@
         <v>2712</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>44873</v>
       </c>
@@ -6190,7 +6193,7 @@
         <v>2691</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>44873</v>
       </c>
@@ -6219,7 +6222,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>44873</v>
       </c>
@@ -6248,7 +6251,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>44873</v>
       </c>
@@ -6277,7 +6280,7 @@
         <v>2829</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>44873</v>
       </c>
@@ -6306,7 +6309,7 @@
         <v>3557</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>44873</v>
       </c>
@@ -6335,7 +6338,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>44873</v>
       </c>
@@ -6364,7 +6367,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>44873</v>
       </c>
@@ -6393,7 +6396,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>44873</v>
       </c>
@@ -6422,7 +6425,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>44873</v>
       </c>
@@ -6451,7 +6454,7 @@
         <v>28956</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>44873</v>
       </c>
@@ -6480,7 +6483,7 @@
         <v>66276</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>44873</v>
       </c>
@@ -6509,7 +6512,7 @@
         <v>82007</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>44873</v>
       </c>
@@ -6538,7 +6541,7 @@
         <v>30871</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>44873</v>
       </c>
@@ -6567,7 +6570,7 @@
         <v>64777</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>44873</v>
       </c>
@@ -6596,7 +6599,7 @@
         <v>46177</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>44873</v>
       </c>
@@ -6625,7 +6628,7 @@
         <v>33017</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>44873</v>
       </c>
@@ -6654,7 +6657,7 @@
         <v>13358</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>44873</v>
       </c>
@@ -6683,7 +6686,7 @@
         <v>35246</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
         <v>44873</v>
       </c>
@@ -6712,7 +6715,7 @@
         <v>41966</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>44873</v>
       </c>
@@ -6741,7 +6744,7 @@
         <v>17362</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
         <v>44873</v>
       </c>
@@ -6770,7 +6773,7 @@
         <v>34487</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
         <v>44873</v>
       </c>
@@ -6799,7 +6802,7 @@
         <v>27598</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
         <v>44873</v>
       </c>
@@ -6828,7 +6831,7 @@
         <v>14746</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
         <v>44873</v>
       </c>
@@ -6857,7 +6860,7 @@
         <v>16907</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
         <v>44873</v>
       </c>
@@ -6886,7 +6889,7 @@
         <v>36880</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
         <v>44873</v>
       </c>
@@ -6915,7 +6918,7 @@
         <v>44492</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
         <v>44873</v>
       </c>
@@ -6944,7 +6947,7 @@
         <v>19627</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
         <v>44873</v>
       </c>
@@ -6973,7 +6976,7 @@
         <v>36607</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
         <v>44873</v>
       </c>
@@ -7002,7 +7005,7 @@
         <v>27370</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
         <v>44873</v>
       </c>
@@ -7031,7 +7034,7 @@
         <v>18222</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
         <v>44873</v>
       </c>
@@ -7060,7 +7063,7 @@
         <v>412417</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>44873</v>
       </c>
@@ -7089,7 +7092,7 @@
         <v>655691</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>44873</v>
       </c>
@@ -7118,7 +7121,7 @@
         <v>780601</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
         <v>44873</v>
       </c>
@@ -7147,7 +7150,7 @@
         <v>415570</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
         <v>44873</v>
       </c>
@@ -7176,7 +7179,7 @@
         <v>673691</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
         <v>44873</v>
       </c>
@@ -7205,7 +7208,7 @@
         <v>613726</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
         <v>44873</v>
       </c>
@@ -7234,7 +7237,7 @@
         <v>404539</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
         <v>44873</v>
       </c>
@@ -7263,7 +7266,7 @@
         <v>80296</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
         <v>44873</v>
       </c>
@@ -7292,7 +7295,7 @@
         <v>130970</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A214" s="1">
         <v>44873</v>
       </c>
@@ -7321,7 +7324,7 @@
         <v>152490</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215" s="1">
         <v>44873</v>
       </c>
@@ -7350,7 +7353,7 @@
         <v>84771</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216" s="1">
         <v>44873</v>
       </c>
@@ -7379,7 +7382,7 @@
         <v>139054</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217" s="1">
         <v>44873</v>
       </c>
@@ -7408,7 +7411,7 @@
         <v>115464</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A218" s="1">
         <v>44873</v>
       </c>
@@ -7437,7 +7440,7 @@
         <v>76800</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A219" s="1">
         <v>44873</v>
       </c>
@@ -7466,7 +7469,7 @@
         <v>3910</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A220" s="1">
         <v>44873</v>
       </c>
@@ -7495,7 +7498,7 @@
         <v>6479</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A221" s="1">
         <v>44873</v>
       </c>
@@ -7524,7 +7527,7 @@
         <v>7455</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A222" s="1">
         <v>44873</v>
       </c>
@@ -7553,7 +7556,7 @@
         <v>3686</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A223" s="1">
         <v>44873</v>
       </c>
@@ -7582,7 +7585,7 @@
         <v>6667</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A224" s="1">
         <v>44873</v>
       </c>
@@ -7611,7 +7614,7 @@
         <v>5474</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225" s="1">
         <v>44873</v>
       </c>
@@ -7640,7 +7643,7 @@
         <v>3635</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226" s="1">
         <v>44873</v>
       </c>
@@ -7669,7 +7672,7 @@
         <v>254691</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227" s="1">
         <v>44873</v>
       </c>
@@ -7698,7 +7701,7 @@
         <v>380142</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228" s="1">
         <v>44873</v>
       </c>
@@ -7727,7 +7730,7 @@
         <v>485891</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229" s="1">
         <v>44873</v>
       </c>
@@ -7756,7 +7759,7 @@
         <v>238831</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230" s="1">
         <v>44873</v>
       </c>
@@ -7785,7 +7788,7 @@
         <v>408811</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231" s="1">
         <v>44873</v>
       </c>
@@ -7814,7 +7817,7 @@
         <v>370669</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232" s="1">
         <v>44873</v>
       </c>
@@ -7843,7 +7846,7 @@
         <v>261834</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233" s="1">
         <v>44873</v>
       </c>
@@ -7872,7 +7875,7 @@
         <v>143182</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234" s="1">
         <v>44873</v>
       </c>
@@ -7901,7 +7904,7 @@
         <v>317951</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A235" s="1">
         <v>44873</v>
       </c>
@@ -7930,7 +7933,7 @@
         <v>389764</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A236" s="1">
         <v>44873</v>
       </c>
@@ -7959,7 +7962,7 @@
         <v>165341</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A237" s="1">
         <v>44873</v>
       </c>
@@ -7988,7 +7991,7 @@
         <v>328053</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238" s="1">
         <v>44873</v>
       </c>
@@ -8017,7 +8020,7 @@
         <v>255413</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239" s="1">
         <v>44873</v>
       </c>
@@ -8046,7 +8049,7 @@
         <v>180618</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A240" s="1">
         <v>44873</v>
       </c>
@@ -8075,7 +8078,7 @@
         <v>6809</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
         <v>44873</v>
       </c>
@@ -8104,7 +8107,7 @@
         <v>12667</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
         <v>44873</v>
       </c>
@@ -8133,7 +8136,7 @@
         <v>15083</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243" s="1">
         <v>44873</v>
       </c>
@@ -8162,7 +8165,7 @@
         <v>7071</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A244" s="1">
         <v>44873</v>
       </c>
@@ -8191,7 +8194,7 @@
         <v>12852</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A245" s="1">
         <v>44873</v>
       </c>
@@ -8220,7 +8223,7 @@
         <v>10760</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A246" s="1">
         <v>44873</v>
       </c>
@@ -8249,7 +8252,7 @@
         <v>7318</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A247" s="1">
         <v>44873</v>
       </c>
@@ -8278,7 +8281,7 @@
         <v>205726</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A248" s="1">
         <v>44873</v>
       </c>
@@ -8307,7 +8310,7 @@
         <v>296880</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A249" s="1">
         <v>44873</v>
       </c>
@@ -8336,7 +8339,7 @@
         <v>365946</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A250" s="1">
         <v>44873</v>
       </c>
@@ -8365,7 +8368,7 @@
         <v>181059</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A251" s="1">
         <v>44873</v>
       </c>
@@ -8394,7 +8397,7 @@
         <v>307993</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252" s="1">
         <v>44873</v>
       </c>
@@ -8423,7 +8426,7 @@
         <v>293539</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253" s="1">
         <v>44873</v>
       </c>
@@ -8452,7 +8455,7 @@
         <v>199471</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254" s="1">
         <v>44873</v>
       </c>
@@ -8481,7 +8484,7 @@
         <v>359290</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A255" s="1">
         <v>44873</v>
       </c>
@@ -8510,7 +8513,7 @@
         <v>612647</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A256" s="1">
         <v>44873</v>
       </c>
@@ -8539,7 +8542,7 @@
         <v>823526</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A257" s="1">
         <v>44873</v>
       </c>
@@ -8568,7 +8571,7 @@
         <v>386977</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A258" s="1">
         <v>44873</v>
       </c>
@@ -8597,7 +8600,7 @@
         <v>693460</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A259" s="1">
         <v>44873</v>
       </c>
@@ -8626,7 +8629,7 @@
         <v>556065</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A260" s="1">
         <v>44873</v>
       </c>
@@ -8655,7 +8658,7 @@
         <v>396976</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A261" s="1">
         <v>44873</v>
       </c>
@@ -8684,7 +8687,7 @@
         <v>31657</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A262" s="1">
         <v>44873</v>
       </c>
@@ -8713,7 +8716,7 @@
         <v>181120</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A263" s="1">
         <v>44873</v>
       </c>
@@ -8742,7 +8745,7 @@
         <v>242820</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A264" s="1">
         <v>44873</v>
       </c>
@@ -8771,7 +8774,7 @@
         <v>62154</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A265" s="1">
         <v>44873</v>
       </c>
@@ -8800,7 +8803,7 @@
         <v>177690</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A266" s="1">
         <v>44873</v>
       </c>
@@ -8829,7 +8832,7 @@
         <v>103165</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A267" s="1">
         <v>44873</v>
       </c>
@@ -8858,7 +8861,7 @@
         <v>62345</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A268" s="1">
         <v>44873</v>
       </c>
@@ -8887,7 +8890,7 @@
         <v>72332</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A269" s="1">
         <v>44873</v>
       </c>
@@ -8916,7 +8919,7 @@
         <v>121361</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A270" s="1">
         <v>44873</v>
       </c>
@@ -8945,7 +8948,7 @@
         <v>143086</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A271" s="1">
         <v>44873</v>
       </c>
@@ -8974,7 +8977,7 @@
         <v>67587</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A272" s="1">
         <v>44873</v>
       </c>
@@ -9003,7 +9006,7 @@
         <v>125379</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A273" s="1">
         <v>44873</v>
       </c>
@@ -9032,7 +9035,7 @@
         <v>107144</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A274" s="1">
         <v>44873</v>
       </c>
@@ -9061,7 +9064,7 @@
         <v>72988</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A275" s="1">
         <v>44873</v>
       </c>
@@ -9090,7 +9093,7 @@
         <v>44830</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A276" s="1">
         <v>44873</v>
       </c>
@@ -9119,7 +9122,7 @@
         <v>81625</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A277" s="1">
         <v>44873</v>
       </c>
@@ -9148,7 +9151,7 @@
         <v>98559</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A278" s="1">
         <v>44873</v>
       </c>
@@ -9177,7 +9180,7 @@
         <v>48485</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A279" s="1">
         <v>44873</v>
       </c>
@@ -9206,7 +9209,7 @@
         <v>88641</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A280" s="1">
         <v>44873</v>
       </c>
@@ -9235,7 +9238,7 @@
         <v>66691</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A281" s="1">
         <v>44873</v>
       </c>
@@ -9264,7 +9267,7 @@
         <v>46602</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A282" s="1">
         <v>44873</v>
       </c>
@@ -9293,7 +9296,7 @@
         <v>49724</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A283" s="1">
         <v>44873</v>
       </c>
@@ -9322,7 +9325,7 @@
         <v>164976</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A284" s="1">
         <v>44873</v>
       </c>
@@ -9351,7 +9354,7 @@
         <v>200867</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A285" s="1">
         <v>44873</v>
       </c>
@@ -9380,7 +9383,7 @@
         <v>74530</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A286" s="1">
         <v>44873</v>
       </c>
@@ -9409,7 +9412,7 @@
         <v>162060</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A287" s="1">
         <v>44873</v>
       </c>
@@ -9438,7 +9441,7 @@
         <v>127000</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A288" s="1">
         <v>44873</v>
       </c>
@@ -9467,7 +9470,7 @@
         <v>62809</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A289" s="1">
         <v>44873</v>
       </c>
@@ -9496,7 +9499,7 @@
         <v>42636</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A290" s="1">
         <v>44873</v>
       </c>
@@ -9525,7 +9528,7 @@
         <v>89657</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A291" s="1">
         <v>44873</v>
       </c>
@@ -9554,7 +9557,7 @@
         <v>110066</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A292" s="1">
         <v>44873</v>
       </c>
@@ -9583,7 +9586,7 @@
         <v>43400</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A293" s="1">
         <v>44873</v>
       </c>
@@ -9612,7 +9615,7 @@
         <v>92911</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A294" s="1">
         <v>44873</v>
       </c>
@@ -9641,7 +9644,7 @@
         <v>72731</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A295" s="1">
         <v>44873</v>
       </c>
@@ -9670,7 +9673,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A296" s="1">
         <v>44873</v>
       </c>
@@ -9699,7 +9702,7 @@
         <v>127939</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A297" s="1">
         <v>44873</v>
       </c>
@@ -9728,7 +9731,7 @@
         <v>355886</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A298" s="1">
         <v>44873</v>
       </c>
@@ -9757,7 +9760,7 @@
         <v>438950</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A299" s="1">
         <v>44873</v>
       </c>
@@ -9786,7 +9789,7 @@
         <v>177866</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A300" s="1">
         <v>44873</v>
       </c>
@@ -9815,7 +9818,7 @@
         <v>348125</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A301" s="1">
         <v>44873</v>
       </c>
@@ -9844,7 +9847,7 @@
         <v>286663</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A302" s="1">
         <v>44873</v>
       </c>
@@ -9873,7 +9876,7 @@
         <v>148137</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A303" s="1">
         <v>44873</v>
       </c>
@@ -9902,7 +9905,7 @@
         <v>19654</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A304" s="1">
         <v>44873</v>
       </c>
@@ -9931,7 +9934,7 @@
         <v>66892</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A305" s="1">
         <v>44873</v>
       </c>
@@ -9960,7 +9963,7 @@
         <v>84910</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A306" s="1">
         <v>44873</v>
       </c>
@@ -9989,7 +9992,7 @@
         <v>26162</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A307" s="1">
         <v>44873</v>
       </c>
@@ -10018,7 +10021,7 @@
         <v>69544</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A308" s="1">
         <v>44873</v>
       </c>
@@ -10047,7 +10050,7 @@
         <v>40039</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A309" s="1">
         <v>44873</v>
       </c>
@@ -10076,7 +10079,7 @@
         <v>28150</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A310" s="1">
         <v>44873</v>
       </c>
@@ -10105,7 +10108,7 @@
         <v>36561</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A311" s="1">
         <v>44873</v>
       </c>
@@ -10134,7 +10137,7 @@
         <v>49914</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A312" s="1">
         <v>44873</v>
       </c>
@@ -10163,7 +10166,7 @@
         <v>57727</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A313" s="1">
         <v>44873</v>
       </c>
@@ -10192,7 +10195,7 @@
         <v>34005</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A314" s="1">
         <v>44873</v>
       </c>
@@ -10221,7 +10224,7 @@
         <v>54888</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A315" s="1">
         <v>44873</v>
       </c>
@@ -10250,7 +10253,7 @@
         <v>47032</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A316" s="1">
         <v>44873</v>
       </c>
@@ -10279,7 +10282,7 @@
         <v>33808</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A317" s="1">
         <v>44873</v>
       </c>
@@ -10308,7 +10311,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A318" s="1">
         <v>44873</v>
       </c>
@@ -10337,7 +10340,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A319" s="1">
         <v>44873</v>
       </c>
@@ -10366,7 +10369,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A320" s="1">
         <v>44873</v>
       </c>
@@ -10395,7 +10398,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A321" s="1">
         <v>44873</v>
       </c>
@@ -10424,7 +10427,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A322" s="1">
         <v>44873</v>
       </c>
@@ -10453,7 +10456,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A323" s="1">
         <v>44873</v>
       </c>
@@ -10482,7 +10485,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A324" s="1">
         <v>44873</v>
       </c>
@@ -10511,7 +10514,7 @@
         <v>8175</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A325" s="1">
         <v>44873</v>
       </c>
@@ -10540,7 +10543,7 @@
         <v>12227</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A326" s="1">
         <v>44873</v>
       </c>
@@ -10569,7 +10572,7 @@
         <v>14685</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A327" s="1">
         <v>44873</v>
       </c>
@@ -10598,7 +10601,7 @@
         <v>7598</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A328" s="1">
         <v>44873</v>
       </c>
@@ -10627,7 +10630,7 @@
         <v>12408</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A329" s="1">
         <v>44873</v>
       </c>
@@ -10656,7 +10659,7 @@
         <v>11086</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A330" s="1">
         <v>44873</v>
       </c>
@@ -10685,7 +10688,7 @@
         <v>7493</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A331" s="1">
         <v>44873</v>
       </c>
@@ -10714,7 +10717,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A332" s="1">
         <v>44873</v>
       </c>
@@ -10743,7 +10746,7 @@
         <v>90011</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A333" s="1">
         <v>44873</v>
       </c>
@@ -10772,7 +10775,7 @@
         <v>108014</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A334" s="1">
         <v>44873</v>
       </c>
@@ -10801,7 +10804,7 @@
         <v>45829</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A335" s="1">
         <v>44873</v>
       </c>
@@ -10830,7 +10833,7 @@
         <v>90724</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A336" s="1">
         <v>44873</v>
       </c>
@@ -10859,7 +10862,7 @@
         <v>77134</v>
       </c>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A337" s="1">
         <v>44873</v>
       </c>
@@ -10888,7 +10891,7 @@
         <v>46824</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A338" s="1">
         <v>44873</v>
       </c>
@@ -10917,7 +10920,7 @@
         <v>40453</v>
       </c>
     </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A339" s="1">
         <v>44873</v>
       </c>
@@ -10946,7 +10949,7 @@
         <v>136195</v>
       </c>
     </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A340" s="1">
         <v>44873</v>
       </c>
@@ -10975,7 +10978,7 @@
         <v>168988</v>
       </c>
     </row>
-    <row r="341" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A341" s="1">
         <v>44873</v>
       </c>
@@ -11004,7 +11007,7 @@
         <v>54412</v>
       </c>
     </row>
-    <row r="342" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A342" s="1">
         <v>44873</v>
       </c>
@@ -11033,7 +11036,7 @@
         <v>135831</v>
       </c>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A343" s="1">
         <v>44873</v>
       </c>
@@ -11062,7 +11065,7 @@
         <v>100703</v>
       </c>
     </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A344" s="1">
         <v>44873</v>
       </c>
@@ -11091,7 +11094,7 @@
         <v>53178</v>
       </c>
     </row>
-    <row r="345" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A345" s="1">
         <v>44873</v>
       </c>
@@ -11120,7 +11123,7 @@
         <v>62830</v>
       </c>
     </row>
-    <row r="346" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A346" s="1">
         <v>44873</v>
       </c>
@@ -11149,7 +11152,7 @@
         <v>92808</v>
       </c>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A347" s="1">
         <v>44873</v>
       </c>
@@ -11178,7 +11181,7 @@
         <v>107048</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A348" s="1">
         <v>44873</v>
       </c>
@@ -11207,7 +11210,7 @@
         <v>53255</v>
       </c>
     </row>
-    <row r="349" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A349" s="1">
         <v>44873</v>
       </c>
@@ -11236,7 +11239,7 @@
         <v>95686</v>
       </c>
     </row>
-    <row r="350" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A350" s="1">
         <v>44873</v>
       </c>
@@ -11265,7 +11268,7 @@
         <v>83285</v>
       </c>
     </row>
-    <row r="351" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A351" s="1">
         <v>44873</v>
       </c>
@@ -11294,7 +11297,7 @@
         <v>58991</v>
       </c>
     </row>
-    <row r="352" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A352" s="1">
         <v>44873</v>
       </c>
@@ -11323,7 +11326,7 @@
         <v>13685</v>
       </c>
     </row>
-    <row r="353" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A353" s="1">
         <v>44873</v>
       </c>
@@ -11352,7 +11355,7 @@
         <v>19577</v>
       </c>
     </row>
-    <row r="354" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A354" s="1">
         <v>44873</v>
       </c>
@@ -11381,7 +11384,7 @@
         <v>22593</v>
       </c>
     </row>
-    <row r="355" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A355" s="1">
         <v>44873</v>
       </c>
@@ -11410,7 +11413,7 @@
         <v>13021</v>
       </c>
     </row>
-    <row r="356" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A356" s="1">
         <v>44873</v>
       </c>
@@ -11439,7 +11442,7 @@
         <v>21137</v>
       </c>
     </row>
-    <row r="357" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A357" s="1">
         <v>44873</v>
       </c>
@@ -11468,7 +11471,7 @@
         <v>19400</v>
       </c>
     </row>
-    <row r="358" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A358" s="1">
         <v>44873</v>
       </c>
@@ -11497,7 +11500,7 @@
         <v>13856</v>
       </c>
     </row>
-    <row r="359" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A359" s="1">
         <v>44873</v>
       </c>
@@ -11526,7 +11529,7 @@
         <v>11199</v>
       </c>
     </row>
-    <row r="360" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A360" s="1">
         <v>44873</v>
       </c>
@@ -11555,7 +11558,7 @@
         <v>15422</v>
       </c>
     </row>
-    <row r="361" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A361" s="1">
         <v>44873</v>
       </c>
@@ -11584,7 +11587,7 @@
         <v>17490</v>
       </c>
     </row>
-    <row r="362" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A362" s="1">
         <v>44873</v>
       </c>
@@ -11613,7 +11616,7 @@
         <v>10651</v>
       </c>
     </row>
-    <row r="363" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A363" s="1">
         <v>44873</v>
       </c>
@@ -11642,7 +11645,7 @@
         <v>16781</v>
       </c>
     </row>
-    <row r="364" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A364" s="1">
         <v>44873</v>
       </c>
@@ -11671,7 +11674,7 @@
         <v>14979</v>
       </c>
     </row>
-    <row r="365" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A365" s="1">
         <v>44873</v>
       </c>
@@ -11700,7 +11703,7 @@
         <v>10858</v>
       </c>
     </row>
-    <row r="366" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A366" s="1">
         <v>44873</v>
       </c>
@@ -11729,7 +11732,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="367" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A367" s="1">
         <v>44873</v>
       </c>
@@ -11758,7 +11761,7 @@
         <v>3136</v>
       </c>
     </row>
-    <row r="368" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A368" s="1">
         <v>44873</v>
       </c>
@@ -11787,7 +11790,7 @@
         <v>3806</v>
       </c>
     </row>
-    <row r="369" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A369" s="1">
         <v>44873</v>
       </c>
@@ -11816,7 +11819,7 @@
         <v>1737</v>
       </c>
     </row>
-    <row r="370" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A370" s="1">
         <v>44873</v>
       </c>
@@ -11845,7 +11848,7 @@
         <v>3479</v>
       </c>
     </row>
-    <row r="371" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A371" s="1">
         <v>44873</v>
       </c>
@@ -11874,7 +11877,7 @@
         <v>2591</v>
       </c>
     </row>
-    <row r="372" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A372" s="1">
         <v>44873</v>
       </c>
@@ -11903,7 +11906,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="373" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A373" s="1">
         <v>44873</v>
       </c>
@@ -11932,7 +11935,7 @@
         <v>48891</v>
       </c>
     </row>
-    <row r="374" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A374" s="1">
         <v>44873</v>
       </c>
@@ -11961,7 +11964,7 @@
         <v>65062</v>
       </c>
     </row>
-    <row r="375" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A375" s="1">
         <v>44873</v>
       </c>
@@ -11990,7 +11993,7 @@
         <v>74970</v>
       </c>
     </row>
-    <row r="376" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A376" s="1">
         <v>44873</v>
       </c>
@@ -12019,7 +12022,7 @@
         <v>41728</v>
       </c>
     </row>
-    <row r="377" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A377" s="1">
         <v>44873</v>
       </c>
@@ -12048,7 +12051,7 @@
         <v>66604</v>
       </c>
     </row>
-    <row r="378" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A378" s="1">
         <v>44873</v>
       </c>
@@ -12077,7 +12080,7 @@
         <v>60131</v>
       </c>
     </row>
-    <row r="379" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A379" s="1">
         <v>44873</v>
       </c>
@@ -12106,7 +12109,7 @@
         <v>46102</v>
       </c>
     </row>
-    <row r="380" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A380" s="1">
         <v>44873</v>
       </c>
@@ -12135,7 +12138,7 @@
         <v>11035</v>
       </c>
     </row>
-    <row r="381" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A381" s="1">
         <v>44873</v>
       </c>
@@ -12164,7 +12167,7 @@
         <v>17215</v>
       </c>
     </row>
-    <row r="382" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A382" s="1">
         <v>44873</v>
       </c>
@@ -12193,7 +12196,7 @@
         <v>20171</v>
       </c>
     </row>
-    <row r="383" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A383" s="1">
         <v>44873</v>
       </c>
@@ -12222,7 +12225,7 @@
         <v>10309</v>
       </c>
     </row>
-    <row r="384" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A384" s="1">
         <v>44873</v>
       </c>
@@ -12251,7 +12254,7 @@
         <v>17874</v>
       </c>
     </row>
-    <row r="385" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A385" s="1">
         <v>44873</v>
       </c>
@@ -12280,7 +12283,7 @@
         <v>14978</v>
       </c>
     </row>
-    <row r="386" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A386" s="1">
         <v>44873</v>
       </c>
@@ -12309,7 +12312,7 @@
         <v>9877</v>
       </c>
     </row>
-    <row r="387" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A387" s="1">
         <v>44873</v>
       </c>
@@ -12338,7 +12341,7 @@
         <v>100532</v>
       </c>
     </row>
-    <row r="388" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A388" s="1">
         <v>44873</v>
       </c>
@@ -12367,7 +12370,7 @@
         <v>188295</v>
       </c>
     </row>
-    <row r="389" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A389" s="1">
         <v>44873</v>
       </c>
@@ -12396,7 +12399,7 @@
         <v>230809</v>
       </c>
     </row>
-    <row r="390" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A390" s="1">
         <v>44873</v>
       </c>
@@ -12425,7 +12428,7 @@
         <v>106580</v>
       </c>
     </row>
-    <row r="391" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A391" s="1">
         <v>44873</v>
       </c>
@@ -12454,7 +12457,7 @@
         <v>187577</v>
       </c>
     </row>
-    <row r="392" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A392" s="1">
         <v>44873</v>
       </c>
@@ -12483,7 +12486,7 @@
         <v>169475</v>
       </c>
     </row>
-    <row r="393" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A393" s="1">
         <v>44873</v>
       </c>
@@ -12512,7 +12515,7 @@
         <v>106357</v>
       </c>
     </row>
-    <row r="394" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A394" s="1">
         <v>44873</v>
       </c>
@@ -12541,7 +12544,7 @@
         <v>17689</v>
       </c>
     </row>
-    <row r="395" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A395" s="1">
         <v>44873</v>
       </c>
@@ -12570,7 +12573,7 @@
         <v>45343</v>
       </c>
     </row>
-    <row r="396" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A396" s="1">
         <v>44873</v>
       </c>
@@ -12599,7 +12602,7 @@
         <v>56317</v>
       </c>
     </row>
-    <row r="397" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A397" s="1">
         <v>44873</v>
       </c>
@@ -12628,7 +12631,7 @@
         <v>20706</v>
       </c>
     </row>
-    <row r="398" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A398" s="1">
         <v>44873</v>
       </c>
@@ -12657,7 +12660,7 @@
         <v>46561</v>
       </c>
     </row>
-    <row r="399" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A399" s="1">
         <v>44873</v>
       </c>
@@ -12686,7 +12689,7 @@
         <v>32984</v>
       </c>
     </row>
-    <row r="400" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A400" s="1">
         <v>44873</v>
       </c>
@@ -12715,7 +12718,7 @@
         <v>20319</v>
       </c>
     </row>
-    <row r="401" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A401" s="1">
         <v>44873</v>
       </c>
@@ -12744,7 +12747,7 @@
         <v>9765</v>
       </c>
     </row>
-    <row r="402" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A402" s="1">
         <v>44873</v>
       </c>
@@ -12773,7 +12776,7 @@
         <v>14429</v>
       </c>
     </row>
-    <row r="403" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A403" s="1">
         <v>44873</v>
       </c>
@@ -12802,7 +12805,7 @@
         <v>16332</v>
       </c>
     </row>
-    <row r="404" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A404" s="1">
         <v>44873</v>
       </c>
@@ -12831,7 +12834,7 @@
         <v>9496</v>
       </c>
     </row>
-    <row r="405" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A405" s="1">
         <v>44873</v>
       </c>
@@ -12860,7 +12863,7 @@
         <v>14859</v>
       </c>
     </row>
-    <row r="406" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A406" s="1">
         <v>44873</v>
       </c>
@@ -12889,7 +12892,7 @@
         <v>13156</v>
       </c>
     </row>
-    <row r="407" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A407" s="1">
         <v>44873</v>
       </c>

</xml_diff>